<commit_message>
Fis some bugs, save data from Choser
</commit_message>
<xml_diff>
--- a/SOURCES/LD_XP.xlsx
+++ b/SOURCES/LD_XP.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si/>
   <si>
     <t>Données de configuration des niveaux joueurs</t>
@@ -68,13 +68,31 @@
     <t>TILE_BAD</t>
   </si>
   <si>
+    <t>Multiplicateur</t>
+  </si>
+  <si>
+    <t>EASY</t>
+  </si>
+  <si>
     <t>EDGE_GOOD</t>
+  </si>
+  <si>
+    <t>EASY_MAX_TILE</t>
+  </si>
+  <si>
+    <t>AGGRESSIVE</t>
   </si>
   <si>
     <t>EASY_MAX_TILE (2)</t>
   </si>
   <si>
+    <t>MINIMAX</t>
+  </si>
+  <si>
     <t>TILE_GOOD</t>
+  </si>
+  <si>
+    <t>CLASSIC</t>
   </si>
   <si>
     <t>AGGRESSIVE (3)</t>
@@ -86,6 +104,9 @@
     <t>CONTINUE_TO_PLAY</t>
   </si>
   <si>
+    <t>Partie perdue</t>
+  </si>
+  <si>
     <t>MINIMAX (4)</t>
   </si>
 </sst>
@@ -93,8 +114,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="0.0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -162,7 +184,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -188,6 +210,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -439,64 +470,64 @@
                   <c:v>10.000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.000000</c:v>
+                  <c:v>26.000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.000000</c:v>
+                  <c:v>50.000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.000000</c:v>
+                  <c:v>82.000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90.000000</c:v>
+                  <c:v>122.000000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>130.000000</c:v>
+                  <c:v>170.000000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>178.000000</c:v>
+                  <c:v>226.000000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>234.000000</c:v>
+                  <c:v>290.000000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>298.000000</c:v>
+                  <c:v>362.000000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>370.000000</c:v>
+                  <c:v>442.000000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>450.000000</c:v>
+                  <c:v>530.000000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>538.000000</c:v>
+                  <c:v>626.000000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>634.000000</c:v>
+                  <c:v>730.000000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>738.000000</c:v>
+                  <c:v>842.000000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>850.000000</c:v>
+                  <c:v>962.000000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>970.000000</c:v>
+                  <c:v>1090.000000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1098.000000</c:v>
+                  <c:v>1226.000000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1234.000000</c:v>
+                  <c:v>1370.000000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1378.000000</c:v>
+                  <c:v>1522.000000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1530.000000</c:v>
+                  <c:v>1682.000000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1690.000000</c:v>
+                  <c:v>1850.000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,8 +626,8 @@
         <c:crossAx val="0"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="450"/>
-        <c:minorUnit val="225"/>
+        <c:majorUnit val="500"/>
+        <c:minorUnit val="250"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -626,14 +657,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>927573</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>190503</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>190504</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1299421</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>66680</xdr:rowOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>66682</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -641,7 +672,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2781773" y="9434831"/>
+        <a:off x="2781773" y="10361296"/>
         <a:ext cx="5421368" cy="3990978"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -1881,7 +1912,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1954,7 +1985,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6">
         <v>10</v>
@@ -1992,20 +2023,20 @@
         <v>1</v>
       </c>
       <c r="B4" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="7">
         <f>$C3+$B4*$D$3</f>
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="7">
         <f>$C4/$K$6</f>
-        <v>0.5625</v>
+        <v>0.8125</v>
       </c>
       <c r="F4" s="7">
         <f>SUM($E$3:E4)</f>
-        <v>0.875</v>
+        <v>1.125</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" t="s" s="7">
@@ -2027,20 +2058,20 @@
         <v>2</v>
       </c>
       <c r="B5" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="6">
         <f>$C4+$B5*$D$3</f>
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="6">
         <f>$C5/$K$6</f>
-        <v>1.0625</v>
+        <v>1.5625</v>
       </c>
       <c r="F5" s="6">
         <f>SUM($E$3:E5)</f>
-        <v>1.9375</v>
+        <v>2.6875</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" t="s" s="6">
@@ -2062,20 +2093,20 @@
         <v>3</v>
       </c>
       <c r="B6" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="7">
         <f>$C5+$B6*$D$3</f>
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7">
         <f>$C6/$K$6</f>
-        <v>1.8125</v>
+        <v>2.5625</v>
       </c>
       <c r="F6" s="7">
         <f>SUM($E$3:E6)</f>
-        <v>3.75</v>
+        <v>5.25</v>
       </c>
       <c r="G6" t="s" s="7">
         <v>16</v>
@@ -2095,20 +2126,20 @@
         <v>4</v>
       </c>
       <c r="B7" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="6">
         <f>$C6+$B7*$D$3</f>
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="6">
         <f>$C7/$K$6</f>
-        <v>2.8125</v>
+        <v>3.8125</v>
       </c>
       <c r="F7" s="6">
         <f>SUM($E$3:E7)</f>
-        <v>6.5625</v>
+        <v>9.0625</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -2121,27 +2152,31 @@
         <v>5</v>
       </c>
       <c r="B8" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="7">
         <f>$C7+$B8*$D$3</f>
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="7">
         <f>$C8/$K$6</f>
-        <v>4.0625</v>
+        <v>5.3125</v>
       </c>
       <c r="F8" s="7">
         <f>SUM($E$3:E8)</f>
-        <v>10.625</v>
+        <v>14.375</v>
       </c>
       <c r="G8" t="s" s="7">
         <v>17</v>
       </c>
       <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="I8" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s" s="7">
+        <v>18</v>
+      </c>
       <c r="K8" s="8"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
@@ -2149,25 +2184,31 @@
         <v>6</v>
       </c>
       <c r="B9" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="6">
         <f>$C8+$B9*$D$3</f>
-        <v>178</v>
+        <v>226</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="6">
         <f>$C9/$K$6</f>
-        <v>5.5625</v>
+        <v>7.0625</v>
       </c>
       <c r="F9" s="6">
         <f>SUM($E$3:E9)</f>
-        <v>16.1875</v>
+        <v>21.4375</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="H9" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
       <c r="K9" s="3"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
@@ -2175,27 +2216,33 @@
         <v>7</v>
       </c>
       <c r="B10" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="7">
         <f>$C9+$B10*$D$3</f>
-        <v>234</v>
+        <v>290</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="7">
         <f>$C10/$K$6</f>
-        <v>7.3125</v>
+        <v>9.0625</v>
       </c>
       <c r="F10" s="7">
         <f>SUM($E$3:E10)</f>
-        <v>23.5</v>
+        <v>30.5</v>
       </c>
       <c r="G10" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="H10" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0</v>
+      </c>
+      <c r="J10" s="8">
+        <v>2</v>
+      </c>
       <c r="K10" s="8"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
@@ -2203,25 +2250,31 @@
         <v>8</v>
       </c>
       <c r="B11" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="6">
         <f>$C10+$B11*$D$3</f>
-        <v>298</v>
+        <v>362</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="6">
         <f>$C11/$K$6</f>
-        <v>9.3125</v>
+        <v>11.3125</v>
       </c>
       <c r="F11" s="6">
         <f>SUM($E$3:E11)</f>
-        <v>32.8125</v>
+        <v>41.8125</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="H11" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2</v>
+      </c>
       <c r="K11" s="3"/>
     </row>
     <row r="12" ht="20.35" customHeight="1">
@@ -2229,27 +2282,33 @@
         <v>9</v>
       </c>
       <c r="B12" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="7">
         <f>$C11+$B12*$D$3</f>
-        <v>370</v>
+        <v>442</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="7">
         <f>$C12/$K$6</f>
-        <v>11.5625</v>
+        <v>13.8125</v>
       </c>
       <c r="F12" s="7">
         <f>SUM($E$3:E12)</f>
-        <v>44.375</v>
+        <v>55.625</v>
       </c>
       <c r="G12" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="H12" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0</v>
+      </c>
+      <c r="J12" s="8">
+        <v>3</v>
+      </c>
       <c r="K12" s="8"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
@@ -2257,27 +2316,33 @@
         <v>10</v>
       </c>
       <c r="B13" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="6">
         <f>$C12+$B13*$D$3</f>
-        <v>450</v>
+        <v>530</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6">
         <f>$C13/$K$6</f>
-        <v>14.0625</v>
+        <v>16.5625</v>
       </c>
       <c r="F13" s="6">
         <f>SUM($E$3:E13)</f>
-        <v>58.4375</v>
+        <v>72.1875</v>
       </c>
       <c r="G13" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="H13" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1</v>
+      </c>
       <c r="K13" s="3"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
@@ -2285,25 +2350,31 @@
         <v>11</v>
       </c>
       <c r="B14" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="7">
         <f>$C13+$B14*$D$3</f>
-        <v>538</v>
+        <v>626</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="7">
         <f>$C14/$K$6</f>
-        <v>16.8125</v>
+        <v>19.5625</v>
       </c>
       <c r="F14" s="7">
         <f>SUM($E$3:E14)</f>
-        <v>75.25</v>
+        <v>91.75</v>
       </c>
       <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="H14" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0</v>
+      </c>
+      <c r="J14" s="8">
+        <v>2</v>
+      </c>
       <c r="K14" s="8"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
@@ -2311,25 +2382,31 @@
         <v>12</v>
       </c>
       <c r="B15" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" s="6">
         <f>$C14+$B15*$D$3</f>
-        <v>634</v>
+        <v>730</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="6">
         <f>$C15/$K$6</f>
-        <v>19.8125</v>
+        <v>22.8125</v>
       </c>
       <c r="F15" s="6">
         <f>SUM($E$3:E15)</f>
-        <v>95.0625</v>
+        <v>114.5625</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="H15" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>2</v>
+      </c>
       <c r="K15" s="3"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
@@ -2337,27 +2414,33 @@
         <v>13</v>
       </c>
       <c r="B16" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="7">
         <f>$C15+$B16*$D$3</f>
-        <v>738</v>
+        <v>842</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="7">
         <f>$C16/$K$6</f>
-        <v>23.0625</v>
+        <v>26.3125</v>
       </c>
       <c r="F16" s="7">
         <f>SUM($E$3:E16)</f>
-        <v>118.125</v>
+        <v>140.875</v>
       </c>
       <c r="G16" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="H16" t="s" s="7">
+        <v>17</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0</v>
+      </c>
+      <c r="J16" s="8">
+        <v>2</v>
+      </c>
       <c r="K16" s="8"/>
     </row>
     <row r="17" ht="20.35" customHeight="1">
@@ -2365,27 +2448,33 @@
         <v>14</v>
       </c>
       <c r="B17" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" s="6">
         <f>$C16+$B17*$D$3</f>
-        <v>850</v>
+        <v>962</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="6">
         <f>$C17/$K$6</f>
-        <v>26.5625</v>
+        <v>30.0625</v>
       </c>
       <c r="F17" s="6">
         <f>SUM($E$3:E17)</f>
-        <v>144.6875</v>
+        <v>170.9375</v>
       </c>
       <c r="G17" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="H17" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3">
+        <v>2</v>
+      </c>
       <c r="K17" s="3"/>
     </row>
     <row r="18" ht="20.35" customHeight="1">
@@ -2393,25 +2482,31 @@
         <v>15</v>
       </c>
       <c r="B18" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="7">
         <f>$C17+$B18*$D$3</f>
-        <v>970</v>
+        <v>1090</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="7">
         <f>$C18/$K$6</f>
-        <v>30.3125</v>
+        <v>34.0625</v>
       </c>
       <c r="F18" s="7">
         <f>SUM($E$3:E18)</f>
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
+      <c r="H18" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0</v>
+      </c>
+      <c r="J18" s="8">
+        <v>3</v>
+      </c>
       <c r="K18" s="8"/>
     </row>
     <row r="19" ht="20.35" customHeight="1">
@@ -2419,51 +2514,63 @@
         <v>16</v>
       </c>
       <c r="B19" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="6">
         <f>$C18+$B19*$D$3</f>
-        <v>1098</v>
+        <v>1226</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="6">
         <f>$C19/$K$6</f>
-        <v>34.3125</v>
+        <v>38.3125</v>
       </c>
       <c r="F19" s="6">
         <f>SUM($E$3:E19)</f>
-        <v>209.3125</v>
+        <v>243.3125</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="H19" t="s" s="6">
+        <v>29</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
+        <v>4</v>
+      </c>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" ht="20.35" customHeight="1">
+    <row r="20" ht="32.25" customHeight="1">
       <c r="A20" s="7">
         <v>17</v>
       </c>
       <c r="B20" s="7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="7">
         <f>$C19+$B20*$D$3</f>
-        <v>1234</v>
+        <v>1370</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="7">
         <f>$C20/$K$6</f>
-        <v>38.5625</v>
+        <v>42.8125</v>
       </c>
       <c r="F20" s="7">
         <f>SUM($E$3:E20)</f>
-        <v>247.875</v>
+        <v>286.125</v>
       </c>
       <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+      <c r="H20" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="I20" s="8">
+        <v>1</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0</v>
+      </c>
       <c r="K20" s="8"/>
     </row>
     <row r="21" ht="20.35" customHeight="1">
@@ -2471,27 +2578,33 @@
         <v>18</v>
       </c>
       <c r="B21" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21" s="6">
         <f>$C20+$B21*$D$3</f>
-        <v>1378</v>
+        <v>1522</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="6">
         <f>$C21/$K$6</f>
-        <v>43.0625</v>
+        <v>47.5625</v>
       </c>
       <c r="F21" s="6">
         <f>SUM($E$3:E21)</f>
-        <v>290.9375</v>
+        <v>333.6875</v>
       </c>
       <c r="G21" t="s" s="6">
-        <v>23</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="H21" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="I21" s="3">
+        <v>10</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
       <c r="K21" s="3"/>
     </row>
     <row r="22" ht="20.35" customHeight="1">
@@ -2499,25 +2612,31 @@
         <v>19</v>
       </c>
       <c r="B22" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C22" s="7">
         <f>$C21+$B22*$D$3</f>
-        <v>1530</v>
+        <v>1682</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="7">
         <f>$C22/$K$6</f>
-        <v>47.8125</v>
+        <v>52.5625</v>
       </c>
       <c r="F22" s="7">
         <f>SUM($E$3:E22)</f>
-        <v>338.75</v>
+        <v>386.25</v>
       </c>
       <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
+      <c r="H22" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="I22" s="8">
+        <v>0</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0.5</v>
+      </c>
       <c r="K22" s="8"/>
     </row>
     <row r="23" ht="20.35" customHeight="1">
@@ -2525,20 +2644,20 @@
         <v>20</v>
       </c>
       <c r="B23" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C23" s="6">
         <f>$C22+$B23*$D$3</f>
-        <v>1690</v>
+        <v>1850</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="6">
         <f>$C23/$K$6</f>
-        <v>52.8125</v>
+        <v>57.8125</v>
       </c>
       <c r="F23" s="6">
         <f>SUM($E$3:E23)</f>
-        <v>391.5625</v>
+        <v>444.0625</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -2551,25 +2670,25 @@
         <v>21</v>
       </c>
       <c r="B24" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C24" s="7">
         <f>$C23+$B24*$D$3</f>
-        <v>1858</v>
+        <v>2026</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="7">
         <f>$C24/$K$6</f>
-        <v>58.0625</v>
+        <v>63.3125</v>
       </c>
       <c r="F24" s="7">
         <f>SUM($E$3:E24)</f>
-        <v>449.625</v>
+        <v>507.375</v>
       </c>
       <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="H24" s="10"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
+      <c r="J24" s="10"/>
       <c r="K24" s="8"/>
     </row>
     <row r="25" ht="20.35" customHeight="1">
@@ -2577,25 +2696,25 @@
         <v>22</v>
       </c>
       <c r="B25" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C25" s="6">
         <f>$C24+$B25*$D$3</f>
-        <v>2034</v>
+        <v>2210</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="6">
         <f>$C25/$K$6</f>
-        <v>63.5625</v>
+        <v>69.0625</v>
       </c>
       <c r="F25" s="6">
         <f>SUM($E$3:E25)</f>
-        <v>513.1875</v>
+        <v>576.4375</v>
       </c>
       <c r="G25" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="H25" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="H25" s="11"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2605,23 +2724,23 @@
         <v>23</v>
       </c>
       <c r="B26" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C26" s="7">
         <f>$C25+$B26*$D$3</f>
-        <v>2218</v>
+        <v>2402</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="7">
         <f>$C26/$K$6</f>
-        <v>69.3125</v>
+        <v>75.0625</v>
       </c>
       <c r="F26" s="7">
         <f>SUM($E$3:E26)</f>
-        <v>582.5</v>
+        <v>651.5</v>
       </c>
       <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
+      <c r="H26" s="10"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -2631,23 +2750,23 @@
         <v>24</v>
       </c>
       <c r="B27" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C27" s="6">
         <f>$C26+$B27*$D$3</f>
-        <v>2410</v>
+        <v>2602</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="6">
         <f>$C27/$K$6</f>
-        <v>75.3125</v>
+        <v>81.3125</v>
       </c>
       <c r="F27" s="6">
         <f>SUM($E$3:E27)</f>
-        <v>657.8125</v>
+        <v>732.8125</v>
       </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="H27" s="11"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2657,23 +2776,23 @@
         <v>25</v>
       </c>
       <c r="B28" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" s="7">
         <f>$C27+$B28*$D$3</f>
-        <v>2610</v>
+        <v>2810</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="7">
         <f>$C28/$K$6</f>
-        <v>81.5625</v>
+        <v>87.8125</v>
       </c>
       <c r="F28" s="7">
         <f>SUM($E$3:E28)</f>
-        <v>739.375</v>
+        <v>820.625</v>
       </c>
       <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
+      <c r="H28" s="10"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
@@ -2683,23 +2802,23 @@
         <v>26</v>
       </c>
       <c r="B29" s="6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="6">
         <f>$C28+$B29*$D$3</f>
-        <v>2818</v>
+        <v>3026</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="6">
         <f>$C29/$K$6</f>
-        <v>88.0625</v>
+        <v>94.5625</v>
       </c>
       <c r="F29" s="6">
         <f>SUM($E$3:E29)</f>
-        <v>827.4375</v>
+        <v>915.1875</v>
       </c>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="H29" s="11"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -2709,23 +2828,23 @@
         <v>27</v>
       </c>
       <c r="B30" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C30" s="7">
         <f>$C29+$B30*$D$3</f>
-        <v>3034</v>
+        <v>3250</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="7">
         <f>$C30/$K$6</f>
-        <v>94.8125</v>
+        <v>101.5625</v>
       </c>
       <c r="F30" s="7">
         <f>SUM($E$3:E30)</f>
-        <v>922.25</v>
+        <v>1016.75</v>
       </c>
       <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
+      <c r="H30" s="10"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
@@ -2735,23 +2854,23 @@
         <v>28</v>
       </c>
       <c r="B31" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C31" s="6">
         <f>$C30+$B31*$D$3</f>
-        <v>3258</v>
+        <v>3482</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="6">
         <f>$C31/$K$6</f>
-        <v>101.8125</v>
+        <v>108.8125</v>
       </c>
       <c r="F31" s="6">
         <f>SUM($E$3:E31)</f>
-        <v>1024.0625</v>
+        <v>1125.5625</v>
       </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="H31" s="11"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2761,23 +2880,23 @@
         <v>29</v>
       </c>
       <c r="B32" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32" s="7">
         <f>$C31+$B32*$D$3</f>
-        <v>3490</v>
+        <v>3722</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="7">
         <f>$C32/$K$6</f>
-        <v>109.0625</v>
+        <v>116.3125</v>
       </c>
       <c r="F32" s="7">
         <f>SUM($E$3:E32)</f>
-        <v>1133.125</v>
+        <v>1241.875</v>
       </c>
       <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
+      <c r="H32" s="10"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
@@ -2787,23 +2906,23 @@
         <v>30</v>
       </c>
       <c r="B33" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C33" s="6">
         <f>$C32+$B33*$D$3</f>
-        <v>3730</v>
+        <v>3970</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="6">
         <f>$C33/$K$6</f>
-        <v>116.5625</v>
+        <v>124.0625</v>
       </c>
       <c r="F33" s="6">
         <f>SUM($E$3:E33)</f>
-        <v>1249.6875</v>
+        <v>1365.9375</v>
       </c>
       <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="H33" s="11"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2813,26 +2932,98 @@
         <v>31</v>
       </c>
       <c r="B34" s="7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C34" s="7">
         <f>$C33+$B34*$D$3</f>
-        <v>3978</v>
+        <v>4226</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="7">
         <f>$C34/$K$6</f>
-        <v>124.3125</v>
+        <v>132.0625</v>
       </c>
       <c r="F34" s="7">
         <f>SUM($E$3:E34)</f>
-        <v>1374</v>
+        <v>1498</v>
       </c>
       <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
+      <c r="H34" s="10"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
+    </row>
+    <row r="35" ht="20.35" customHeight="1">
+      <c r="A35" s="11"/>
+      <c r="B35" s="6">
+        <v>33</v>
+      </c>
+      <c r="C35" s="6">
+        <f>$C34+$B35*$D$3</f>
+        <v>4490</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="6">
+        <f>$C35/$K$6</f>
+        <v>140.3125</v>
+      </c>
+      <c r="F35" s="6">
+        <f>SUM($E$3:E35)</f>
+        <v>1638.3125</v>
+      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" ht="20.35" customHeight="1">
+      <c r="A36" s="10"/>
+      <c r="B36" s="7">
+        <v>34</v>
+      </c>
+      <c r="C36" s="7">
+        <f>$C35+$B36*$D$3</f>
+        <v>4762</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="7">
+        <f>$C36/$K$6</f>
+        <v>148.8125</v>
+      </c>
+      <c r="F36" s="7">
+        <f>SUM($E$3:E36)</f>
+        <v>1787.125</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+    </row>
+    <row r="37" ht="20.35" customHeight="1">
+      <c r="A37" s="11"/>
+      <c r="B37" s="6">
+        <v>35</v>
+      </c>
+      <c r="C37" s="6">
+        <f>$C36+$B37*$D$3</f>
+        <v>5042</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="6">
+        <f>$C37/$K$6</f>
+        <v>157.5625</v>
+      </c>
+      <c r="F37" s="6">
+        <f>SUM($E$3:E37)</f>
+        <v>1944.6875</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>